<commit_message>
IGAC y SGC en un solo codigo
</commit_message>
<xml_diff>
--- a/EstadoestacionesSGC.xlsx
+++ b/EstadoestacionesSGC.xlsx
@@ -36448,7 +36448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG109"/>
+  <dimension ref="A1:AH109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36497,125 +36497,130 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>068</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>069</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>070</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>071</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>072</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>073</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>074</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>075</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>076</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>077</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>078</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>079</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>080</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>081</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>082</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>083</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>084</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>085</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>086</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>087</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>088</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>089</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>090</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>091</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
@@ -36664,125 +36669,130 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>068</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>069</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>070</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>071</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>072</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>073</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>074</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>075</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>076</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>077</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>078</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>079</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>080</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>081</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>082</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>083</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>084</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>085</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>086</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>087</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>088</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>089</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>090</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>091</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>Total Rinex</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
@@ -36831,125 +36841,130 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>(2304, 5)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>(2304, 6)</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>(2305, 0)</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>(2305, 1)</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>(2305, 2)</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>(2305, 3)</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>(2305, 4)</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>(2305, 5)</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>(2305, 6)</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>(2306, 0)</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>(2306, 1)</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>(2306, 2)</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>(2306, 3)</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>(2306, 4)</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>(2306, 5)</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>(2306, 6)</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>(2307, 0)</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>(2307, 1)</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>(2307, 2)</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>(2307, 3)</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>(2307, 4)</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>(2307, 5)</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>(2307, 6)</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AF3" t="inlineStr">
         <is>
           <t>(2308, 0)</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr">
+      <c r="AG3" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="AG3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -37113,10 +37128,15 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
           <t> </t>
         </is>
       </c>
-      <c r="AG4" t="inlineStr">
+      <c r="AH4" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -37278,10 +37298,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG5" t="n">
         <v>0</v>
       </c>
-      <c r="AG5" t="inlineStr">
+      <c r="AH5" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -37335,7 +37360,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -37443,10 +37468,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF6" t="n">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG6" t="n">
         <v>24</v>
       </c>
-      <c r="AG6" t="inlineStr">
+      <c r="AH6" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -37530,12 +37560,12 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -37608,10 +37638,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF7" t="n">
-        <v>28</v>
-      </c>
-      <c r="AG7" t="inlineStr">
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG7" t="n">
+        <v>29</v>
+      </c>
+      <c r="AH7" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -37773,10 +37808,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF8" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG8" t="inlineStr">
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG8" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH8" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -37860,7 +37900,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -37870,7 +37910,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -37890,7 +37930,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -37910,7 +37950,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
@@ -37938,10 +37978,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF9" t="n">
-        <v>21</v>
-      </c>
-      <c r="AG9" t="inlineStr">
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG9" t="n">
+        <v>22</v>
+      </c>
+      <c r="AH9" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -38103,10 +38148,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF10" t="n">
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG10" t="n">
         <v>0</v>
       </c>
-      <c r="AG10" t="inlineStr">
+      <c r="AH10" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -38268,10 +38318,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF11" t="n">
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG11" t="n">
         <v>0</v>
       </c>
-      <c r="AG11" t="inlineStr">
+      <c r="AH11" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -38355,12 +38410,12 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -38390,12 +38445,12 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -38433,10 +38488,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF12" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG12" t="inlineStr">
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG12" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH12" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -38598,10 +38658,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF13" t="n">
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG13" t="n">
         <v>0</v>
       </c>
-      <c r="AG13" t="inlineStr">
+      <c r="AH13" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -38685,12 +38750,12 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -38715,12 +38780,12 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
@@ -38763,10 +38828,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF14" t="n">
-        <v>26</v>
-      </c>
-      <c r="AG14" t="inlineStr">
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG14" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH14" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -38928,10 +38998,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF15" t="n">
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG15" t="n">
         <v>0</v>
       </c>
-      <c r="AG15" t="inlineStr">
+      <c r="AH15" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -39050,7 +39125,7 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
@@ -39060,27 +39135,27 @@
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD16" t="inlineStr">
@@ -39093,10 +39168,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF16" t="n">
-        <v>26</v>
-      </c>
-      <c r="AG16" t="inlineStr">
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG16" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH16" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -39258,10 +39338,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF17" t="n">
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG17" t="n">
         <v>0</v>
       </c>
-      <c r="AG17" t="inlineStr">
+      <c r="AH17" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -39423,10 +39508,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF18" t="n">
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG18" t="n">
         <v>0</v>
       </c>
-      <c r="AG18" t="inlineStr">
+      <c r="AH18" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -39515,12 +39605,12 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -39588,10 +39678,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF19" t="n">
-        <v>28</v>
-      </c>
-      <c r="AG19" t="inlineStr">
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG19" t="n">
+        <v>29</v>
+      </c>
+      <c r="AH19" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -39753,10 +39848,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF20" t="n">
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG20" t="n">
         <v>0</v>
       </c>
-      <c r="AG20" t="inlineStr">
+      <c r="AH20" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -39918,10 +40018,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF21" t="n">
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG21" t="n">
         <v>0</v>
       </c>
-      <c r="AG21" t="inlineStr">
+      <c r="AH21" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -40015,12 +40120,12 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
@@ -40030,12 +40135,12 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -40045,12 +40150,12 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
@@ -40065,12 +40170,12 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD22" t="inlineStr">
@@ -40083,10 +40188,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF22" t="n">
-        <v>25</v>
-      </c>
-      <c r="AG22" t="inlineStr">
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG22" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH22" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -40248,10 +40358,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF23" t="n">
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG23" t="n">
         <v>0</v>
       </c>
-      <c r="AG23" t="inlineStr">
+      <c r="AH23" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -40413,10 +40528,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF24" t="n">
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG24" t="n">
         <v>0</v>
       </c>
-      <c r="AG24" t="inlineStr">
+      <c r="AH24" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -40578,10 +40698,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF25" t="n">
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG25" t="n">
         <v>0</v>
       </c>
-      <c r="AG25" t="inlineStr">
+      <c r="AH25" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -40743,10 +40868,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF26" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG26" t="inlineStr">
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG26" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH26" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -40908,10 +41038,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF27" t="n">
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG27" t="n">
         <v>0</v>
       </c>
-      <c r="AG27" t="inlineStr">
+      <c r="AH27" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -41073,10 +41208,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF28" t="n">
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG28" t="n">
         <v>0</v>
       </c>
-      <c r="AG28" t="inlineStr">
+      <c r="AH28" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -41238,10 +41378,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF29" t="n">
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG29" t="n">
         <v>0</v>
       </c>
-      <c r="AG29" t="inlineStr">
+      <c r="AH29" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -41403,10 +41548,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF30" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG30" t="inlineStr">
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG30" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH30" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -41550,7 +41700,7 @@
       </c>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr">
@@ -41568,10 +41718,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF31" t="n">
-        <v>25</v>
-      </c>
-      <c r="AG31" t="inlineStr">
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG31" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH31" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -41733,10 +41888,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF32" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG32" t="inlineStr">
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG32" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH32" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -41898,10 +42058,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF33" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG33" t="inlineStr">
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG33" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH33" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -42063,10 +42228,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF34" t="n">
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG34" t="n">
         <v>0</v>
       </c>
-      <c r="AG34" t="inlineStr">
+      <c r="AH34" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -42228,10 +42398,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF35" t="n">
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG35" t="n">
         <v>0</v>
       </c>
-      <c r="AG35" t="inlineStr">
+      <c r="AH35" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -42393,10 +42568,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF36" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG36" t="inlineStr">
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG36" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH36" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -42558,10 +42738,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF37" t="n">
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG37" t="n">
         <v>0</v>
       </c>
-      <c r="AG37" t="inlineStr">
+      <c r="AH37" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -42723,10 +42908,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF38" t="n">
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG38" t="n">
         <v>0</v>
       </c>
-      <c r="AG38" t="inlineStr">
+      <c r="AH38" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -42815,12 +43005,12 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -42888,10 +43078,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF39" t="n">
-        <v>28</v>
-      </c>
-      <c r="AG39" t="inlineStr">
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG39" t="n">
+        <v>29</v>
+      </c>
+      <c r="AH39" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -43053,10 +43248,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF40" t="n">
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG40" t="n">
         <v>0</v>
       </c>
-      <c r="AG40" t="inlineStr">
+      <c r="AH40" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -43218,10 +43418,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF41" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG41" t="inlineStr">
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG41" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH41" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -43383,10 +43588,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF42" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG42" t="inlineStr">
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG42" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH42" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -43548,10 +43758,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF43" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG43" t="inlineStr">
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG43" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH43" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -43713,10 +43928,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF44" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG44" t="inlineStr">
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG44" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH44" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -43765,7 +43985,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -43780,12 +44000,12 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -43795,7 +44015,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -43820,7 +44040,7 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U45" t="inlineStr">
@@ -43830,7 +44050,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W45" t="inlineStr">
@@ -43840,17 +44060,17 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
@@ -43860,17 +44080,17 @@
       </c>
       <c r="AB45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AC45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AE45" t="inlineStr">
@@ -43878,10 +44098,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF45" t="n">
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG45" t="n">
         <v>13</v>
       </c>
-      <c r="AG45" t="inlineStr">
+      <c r="AH45" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -44043,10 +44268,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF46" t="n">
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG46" t="n">
         <v>0</v>
       </c>
-      <c r="AG46" t="inlineStr">
+      <c r="AH46" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -44208,10 +44438,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF47" t="n">
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG47" t="n">
         <v>0</v>
       </c>
-      <c r="AG47" t="inlineStr">
+      <c r="AH47" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -44295,12 +44530,12 @@
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -44320,7 +44555,7 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
@@ -44373,10 +44608,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF48" t="n">
-        <v>15</v>
-      </c>
-      <c r="AG48" t="inlineStr">
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG48" t="n">
+        <v>16</v>
+      </c>
+      <c r="AH48" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -44538,10 +44778,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF49" t="n">
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG49" t="n">
         <v>0</v>
       </c>
-      <c r="AG49" t="inlineStr">
+      <c r="AH49" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -44640,7 +44885,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T50" t="inlineStr">
@@ -44703,10 +44948,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF50" t="n">
-        <v>17</v>
-      </c>
-      <c r="AG50" t="inlineStr">
+      <c r="AF50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG50" t="n">
+        <v>18</v>
+      </c>
+      <c r="AH50" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -44868,10 +45118,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF51" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG51" t="inlineStr">
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG51" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH51" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -44920,7 +45175,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -45033,10 +45288,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF52" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG52" t="inlineStr">
+      <c r="AF52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG52" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH52" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -45198,10 +45458,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF53" t="n">
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG53" t="n">
         <v>0</v>
       </c>
-      <c r="AG53" t="inlineStr">
+      <c r="AH53" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -45265,12 +45530,12 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -45310,12 +45575,12 @@
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W54" t="inlineStr">
@@ -45363,10 +45628,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF54" t="n">
-        <v>25</v>
-      </c>
-      <c r="AG54" t="inlineStr">
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG54" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH54" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -45528,10 +45798,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF55" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG55" t="inlineStr">
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG55" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH55" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -45693,10 +45968,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF56" t="n">
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG56" t="n">
         <v>0</v>
       </c>
-      <c r="AG56" t="inlineStr">
+      <c r="AH56" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -45750,17 +46030,17 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
@@ -45780,7 +46060,7 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
@@ -45790,7 +46070,7 @@
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S57" t="inlineStr">
@@ -45835,7 +46115,7 @@
       </c>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AB57" t="inlineStr">
@@ -45858,10 +46138,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF57" t="n">
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG57" t="n">
         <v>17</v>
       </c>
-      <c r="AG57" t="inlineStr">
+      <c r="AH57" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -46023,10 +46308,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF58" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG58" t="inlineStr">
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG58" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH58" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -46188,10 +46478,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF59" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG59" t="inlineStr">
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG59" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH59" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -46353,10 +46648,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF60" t="n">
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG60" t="n">
         <v>0</v>
       </c>
-      <c r="AG60" t="inlineStr">
+      <c r="AH60" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -46518,10 +46818,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF61" t="n">
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG61" t="n">
         <v>0</v>
       </c>
-      <c r="AG61" t="inlineStr">
+      <c r="AH61" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -46683,10 +46988,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF62" t="n">
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG62" t="n">
         <v>0</v>
       </c>
-      <c r="AG62" t="inlineStr">
+      <c r="AH62" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -46780,7 +47090,7 @@
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S63" t="inlineStr">
@@ -46848,10 +47158,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF63" t="n">
-        <v>12</v>
-      </c>
-      <c r="AG63" t="inlineStr">
+      <c r="AF63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG63" t="n">
+        <v>13</v>
+      </c>
+      <c r="AH63" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -47013,10 +47328,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF64" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG64" t="inlineStr">
+      <c r="AF64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG64" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH64" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -47178,10 +47498,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF65" t="n">
+      <c r="AF65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG65" t="n">
         <v>0</v>
       </c>
-      <c r="AG65" t="inlineStr">
+      <c r="AH65" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -47255,7 +47580,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
@@ -47275,7 +47600,7 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
@@ -47290,12 +47615,12 @@
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
@@ -47315,12 +47640,12 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB66" t="inlineStr">
@@ -47335,18 +47660,23 @@
       </c>
       <c r="AD66" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AE66" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF66" t="n">
-        <v>17</v>
-      </c>
-      <c r="AG66" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG66" t="n">
+        <v>18</v>
+      </c>
+      <c r="AH66" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -47425,7 +47755,7 @@
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -47435,7 +47765,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -47508,10 +47838,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF67" t="n">
-        <v>26</v>
-      </c>
-      <c r="AG67" t="inlineStr">
+      <c r="AF67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG67" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH67" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -47610,12 +47945,12 @@
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
@@ -47625,12 +47960,12 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X68" t="inlineStr">
@@ -47640,7 +47975,7 @@
       </c>
       <c r="Y68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Z68" t="inlineStr">
@@ -47650,7 +47985,7 @@
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AB68" t="inlineStr">
@@ -47670,13 +48005,18 @@
       </c>
       <c r="AE68" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF68" t="n">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG68" t="n">
         <v>6</v>
       </c>
-      <c r="AG68" t="inlineStr">
+      <c r="AH68" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -47838,10 +48178,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF69" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG69" t="inlineStr">
+      <c r="AF69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG69" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH69" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48003,10 +48348,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF70" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG70" t="inlineStr">
+      <c r="AF70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG70" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH70" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48100,7 +48450,7 @@
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S71" t="inlineStr">
@@ -48145,7 +48495,7 @@
       </c>
       <c r="AA71" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB71" t="inlineStr">
@@ -48168,10 +48518,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF71" t="n">
-        <v>16</v>
-      </c>
-      <c r="AG71" t="inlineStr">
+      <c r="AF71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG71" t="n">
+        <v>17</v>
+      </c>
+      <c r="AH71" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48285,12 +48640,12 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X72" t="inlineStr">
@@ -48333,10 +48688,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF72" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG72" t="inlineStr">
+      <c r="AF72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG72" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH72" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48498,10 +48858,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF73" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG73" t="inlineStr">
+      <c r="AF73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG73" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH73" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48610,12 +48975,12 @@
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W74" t="inlineStr">
@@ -48663,10 +49028,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF74" t="n">
-        <v>29</v>
-      </c>
-      <c r="AG74" t="inlineStr">
+      <c r="AF74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG74" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH74" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48730,12 +49100,12 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
@@ -48805,7 +49175,7 @@
       </c>
       <c r="AA75" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AB75" t="inlineStr">
@@ -48828,10 +49198,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF75" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG75" t="inlineStr">
+      <c r="AF75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG75" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH75" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -48993,10 +49368,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF76" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG76" t="inlineStr">
+      <c r="AF76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG76" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH76" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -49055,7 +49435,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -49100,7 +49480,7 @@
       </c>
       <c r="T77" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U77" t="inlineStr">
@@ -49130,7 +49510,7 @@
       </c>
       <c r="Z77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA77" t="inlineStr">
@@ -49158,10 +49538,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF77" t="n">
+      <c r="AF77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG77" t="n">
         <v>16</v>
       </c>
-      <c r="AG77" t="inlineStr">
+      <c r="AH77" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -49260,12 +49645,12 @@
       </c>
       <c r="S78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T78" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U78" t="inlineStr">
@@ -49290,17 +49675,17 @@
       </c>
       <c r="Y78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB78" t="inlineStr">
@@ -49310,7 +49695,7 @@
       </c>
       <c r="AC78" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AD78" t="inlineStr">
@@ -49323,10 +49708,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF78" t="n">
+      <c r="AF78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG78" t="n">
         <v>4</v>
       </c>
-      <c r="AG78" t="inlineStr">
+      <c r="AH78" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -49410,7 +49800,7 @@
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr">
@@ -49420,7 +49810,7 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S79" t="inlineStr">
@@ -49445,12 +49835,12 @@
       </c>
       <c r="W79" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X79" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y79" t="inlineStr">
@@ -49488,10 +49878,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF79" t="n">
-        <v>24</v>
-      </c>
-      <c r="AG79" t="inlineStr">
+      <c r="AF79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG79" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH79" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -49615,7 +50010,7 @@
       </c>
       <c r="X80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Y80" t="inlineStr">
@@ -49653,10 +50048,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF80" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG80" t="inlineStr">
+      <c r="AF80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG80" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH80" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -49818,10 +50218,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF81" t="n">
+      <c r="AF81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG81" t="n">
         <v>0</v>
       </c>
-      <c r="AG81" t="inlineStr">
+      <c r="AH81" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -49983,10 +50388,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF82" t="n">
+      <c r="AF82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG82" t="n">
         <v>0</v>
       </c>
-      <c r="AG82" t="inlineStr">
+      <c r="AH82" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -50070,12 +50480,12 @@
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -50148,10 +50558,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF83" t="n">
-        <v>28</v>
-      </c>
-      <c r="AG83" t="inlineStr">
+      <c r="AF83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG83" t="n">
+        <v>29</v>
+      </c>
+      <c r="AH83" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -50313,10 +50728,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF84" t="n">
+      <c r="AF84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG84" t="n">
         <v>0</v>
       </c>
-      <c r="AG84" t="inlineStr">
+      <c r="AH84" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -50400,12 +50820,12 @@
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -50478,10 +50898,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF85" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG85" t="inlineStr">
+      <c r="AF85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG85" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH85" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -50643,10 +51068,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF86" t="n">
+      <c r="AF86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG86" t="n">
         <v>0</v>
       </c>
-      <c r="AG86" t="inlineStr">
+      <c r="AH86" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -50695,12 +51125,12 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -50808,10 +51238,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF87" t="n">
-        <v>26</v>
-      </c>
-      <c r="AG87" t="inlineStr">
+      <c r="AF87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG87" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH87" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -50895,12 +51330,12 @@
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -50915,7 +51350,7 @@
       </c>
       <c r="T88" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U88" t="inlineStr">
@@ -50973,10 +51408,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF88" t="n">
-        <v>11</v>
-      </c>
-      <c r="AG88" t="inlineStr">
+      <c r="AF88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG88" t="n">
+        <v>12</v>
+      </c>
+      <c r="AH88" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -51138,10 +51578,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF89" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG89" t="inlineStr">
+      <c r="AF89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG89" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH89" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -51303,10 +51748,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF90" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG90" t="inlineStr">
+      <c r="AF90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG90" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH90" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -51468,10 +51918,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF91" t="n">
+      <c r="AF91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG91" t="n">
         <v>0</v>
       </c>
-      <c r="AG91" t="inlineStr">
+      <c r="AH91" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -51633,10 +52088,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF92" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG92" t="inlineStr">
+      <c r="AF92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG92" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH92" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -51700,12 +52160,12 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -51715,12 +52175,12 @@
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
@@ -51798,10 +52258,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF93" t="n">
-        <v>25</v>
-      </c>
-      <c r="AG93" t="inlineStr">
+      <c r="AF93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG93" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH93" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -51963,10 +52428,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF94" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG94" t="inlineStr">
+      <c r="AF94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG94" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH94" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -52128,10 +52598,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF95" t="n">
+      <c r="AF95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG95" t="n">
         <v>0</v>
       </c>
-      <c r="AG95" t="inlineStr">
+      <c r="AH95" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -52293,10 +52768,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF96" t="n">
+      <c r="AF96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG96" t="n">
         <v>0</v>
       </c>
-      <c r="AG96" t="inlineStr">
+      <c r="AH96" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -52458,10 +52938,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF97" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG97" t="inlineStr">
+      <c r="AF97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG97" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH97" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -52525,12 +53010,12 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N98" t="inlineStr">
@@ -52545,7 +53030,7 @@
       </c>
       <c r="P98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q98" t="inlineStr">
@@ -52555,7 +53040,7 @@
       </c>
       <c r="R98" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S98" t="inlineStr">
@@ -52575,12 +53060,12 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W98" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X98" t="inlineStr">
@@ -52623,10 +53108,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF98" t="n">
-        <v>23</v>
-      </c>
-      <c r="AG98" t="inlineStr">
+      <c r="AF98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG98" t="n">
+        <v>24</v>
+      </c>
+      <c r="AH98" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -52715,12 +53205,12 @@
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S99" t="inlineStr">
@@ -52788,10 +53278,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF99" t="n">
-        <v>26</v>
-      </c>
-      <c r="AG99" t="inlineStr">
+      <c r="AF99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG99" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH99" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -52840,7 +53335,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -52875,7 +53370,7 @@
       </c>
       <c r="P100" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q100" t="inlineStr">
@@ -52895,7 +53390,7 @@
       </c>
       <c r="T100" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U100" t="inlineStr">
@@ -52925,7 +53420,7 @@
       </c>
       <c r="Z100" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA100" t="inlineStr">
@@ -52945,7 +53440,7 @@
       </c>
       <c r="AD100" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AE100" t="inlineStr">
@@ -52953,10 +53448,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF100" t="n">
+      <c r="AF100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG100" t="n">
         <v>16</v>
       </c>
-      <c r="AG100" t="inlineStr">
+      <c r="AH100" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -53118,10 +53618,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF101" t="n">
+      <c r="AF101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG101" t="n">
         <v>0</v>
       </c>
-      <c r="AG101" t="inlineStr">
+      <c r="AH101" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -53283,10 +53788,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF102" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG102" t="inlineStr">
+      <c r="AF102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG102" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH102" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -53448,10 +53958,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF103" t="n">
+      <c r="AF103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG103" t="n">
         <v>0</v>
       </c>
-      <c r="AG103" t="inlineStr">
+      <c r="AH103" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -53613,10 +54128,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF104" t="n">
-        <v>26</v>
-      </c>
-      <c r="AG104" t="inlineStr">
+      <c r="AF104" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG104" t="n">
+        <v>27</v>
+      </c>
+      <c r="AH104" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -53778,10 +54298,15 @@
           <t>0</t>
         </is>
       </c>
-      <c r="AF105" t="n">
+      <c r="AF105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG105" t="n">
         <v>0</v>
       </c>
-      <c r="AG105" t="inlineStr">
+      <c r="AH105" t="inlineStr">
         <is>
           <t>Inactiva</t>
         </is>
@@ -53895,12 +54420,12 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W106" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="X106" t="inlineStr">
@@ -53943,10 +54468,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF106" t="n">
-        <v>28</v>
-      </c>
-      <c r="AG106" t="inlineStr">
+      <c r="AF106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG106" t="n">
+        <v>29</v>
+      </c>
+      <c r="AH106" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -54108,10 +54638,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF107" t="n">
-        <v>27</v>
-      </c>
-      <c r="AG107" t="inlineStr">
+      <c r="AF107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG107" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH107" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -54175,12 +54710,12 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -54190,7 +54725,7 @@
       </c>
       <c r="O108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P108" t="inlineStr">
@@ -54200,7 +54735,7 @@
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R108" t="inlineStr">
@@ -54230,12 +54765,12 @@
       </c>
       <c r="W108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X108" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y108" t="inlineStr">
@@ -54265,18 +54800,23 @@
       </c>
       <c r="AD108" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AE108" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF108" t="n">
-        <v>20</v>
-      </c>
-      <c r="AG108" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG108" t="n">
+        <v>21</v>
+      </c>
+      <c r="AH108" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>
@@ -54345,7 +54885,7 @@
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N109" t="inlineStr">
@@ -54438,10 +54978,15 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AF109" t="n">
+      <c r="AF109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG109" t="n">
         <v>19</v>
       </c>
-      <c r="AG109" t="inlineStr">
+      <c r="AH109" t="inlineStr">
         <is>
           <t>Activa</t>
         </is>

</xml_diff>